<commit_message>
latest results and test_dis1 for sched and non sched
</commit_message>
<xml_diff>
--- a/FinalResults-dataport.xlsx
+++ b/FinalResults-dataport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="306" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="291" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="testing more summarized" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="49">
   <si>
     <t>Sabina</t>
   </si>
@@ -176,7 +176,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -220,12 +220,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -297,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,6 +377,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,7 +508,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart473.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -674,7 +672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart474.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -838,7 +836,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart475.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1002,7 +1000,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart476.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1166,7 +1164,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart477.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1330,7 +1328,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart478.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1494,7 +1492,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart479.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1658,7 +1656,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart480.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1822,7 +1820,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart481.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1986,7 +1984,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart482.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2150,7 +2148,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart483.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2364,7 +2362,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart484.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2578,7 +2576,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart485.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2792,7 +2790,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart486.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3006,7 +3004,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart487.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3220,7 +3218,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart488.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3434,7 +3432,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart489.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3648,7 +3646,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart490.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3862,7 +3860,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart491.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4076,7 +4074,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart492.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4290,7 +4288,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart493.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4531,7 +4529,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart494.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4772,7 +4770,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart495.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5013,7 +5011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart496.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5254,7 +5252,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart497.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5495,7 +5493,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart498.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5676,7 +5674,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart499.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5857,7 +5855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart500.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6038,7 +6036,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart501.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6219,7 +6217,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart502.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -6405,15 +6403,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>628560</xdr:colOff>
+      <xdr:colOff>655560</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>699840</xdr:colOff>
+      <xdr:colOff>726480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6421,8 +6419,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6212520" y="4784040"/>
-        <a:ext cx="2509560" cy="1207440"/>
+        <a:off x="6239520" y="4775040"/>
+        <a:ext cx="2509200" cy="1207080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6435,15 +6433,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>686520</xdr:colOff>
+      <xdr:colOff>713520</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
+      <xdr:colOff>716760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6451,8 +6449,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6270480" y="6376320"/>
-        <a:ext cx="2441880" cy="1308600"/>
+        <a:off x="6297480" y="6367320"/>
+        <a:ext cx="2441520" cy="1308240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6465,15 +6463,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>91080</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:colOff>118080</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>719640</xdr:colOff>
+      <xdr:colOff>746280</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6481,8 +6479,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8926200" y="4719960"/>
-        <a:ext cx="2254320" cy="1292760"/>
+        <a:off x="8953200" y="4710960"/>
+        <a:ext cx="2253960" cy="1292400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6495,15 +6493,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>122760</xdr:colOff>
+      <xdr:colOff>149760</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6511,8 +6509,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8957880" y="6325200"/>
-        <a:ext cx="2369160" cy="1303920"/>
+        <a:off x="8984880" y="6316200"/>
+        <a:ext cx="2368800" cy="1303560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6525,15 +6523,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>138240</xdr:colOff>
+      <xdr:colOff>165240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6541,8 +6539,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11412000" y="4750560"/>
-        <a:ext cx="2353320" cy="1380240"/>
+        <a:off x="11439000" y="4741560"/>
+        <a:ext cx="2352960" cy="1379880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6555,15 +6553,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>163800</xdr:colOff>
+      <xdr:colOff>190800</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>42840</xdr:colOff>
+      <xdr:colOff>69480</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6571,8 +6569,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11437560" y="6325200"/>
-        <a:ext cx="2317320" cy="1293840"/>
+        <a:off x="11464560" y="6316200"/>
+        <a:ext cx="2316960" cy="1293480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6585,15 +6583,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>289080</xdr:colOff>
+      <xdr:colOff>316080</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>122040</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6601,8 +6599,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14001120" y="4730400"/>
-        <a:ext cx="2244600" cy="1374120"/>
+        <a:off x="14028120" y="4721400"/>
+        <a:ext cx="2244240" cy="1373760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6615,15 +6613,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>74520</xdr:colOff>
+      <xdr:colOff>101160</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>141480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6631,8 +6629,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13959360" y="6366240"/>
-        <a:ext cx="2265480" cy="1252800"/>
+        <a:off x="13986360" y="6357240"/>
+        <a:ext cx="2265120" cy="1252440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6645,15 +6643,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>375480</xdr:colOff>
+      <xdr:colOff>402120</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>99720</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6661,8 +6659,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16366320" y="4723200"/>
-        <a:ext cx="2598120" cy="1391040"/>
+        <a:off x="16393320" y="4714200"/>
+        <a:ext cx="2597760" cy="1390680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6675,15 +6673,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>281520</xdr:colOff>
+      <xdr:colOff>308520</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>375120</xdr:colOff>
+      <xdr:colOff>401760</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6691,8 +6689,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16431840" y="6254280"/>
-        <a:ext cx="2532240" cy="1366920"/>
+        <a:off x="16458840" y="6245280"/>
+        <a:ext cx="2531880" cy="1366560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6705,15 +6703,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>59400</xdr:colOff>
+      <xdr:colOff>86400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>118080</xdr:colOff>
+      <xdr:colOff>144720</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6721,8 +6719,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13771440" y="9448560"/>
-        <a:ext cx="2496960" cy="1398960"/>
+        <a:off x="13798440" y="9439560"/>
+        <a:ext cx="2496600" cy="1398600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6735,15 +6733,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>71640</xdr:colOff>
+      <xdr:colOff>98640</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
+      <xdr:colOff>154080</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6751,8 +6749,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13783680" y="13393440"/>
-        <a:ext cx="2494080" cy="1426320"/>
+        <a:off x="13810680" y="13384440"/>
+        <a:ext cx="2493720" cy="1425960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6765,15 +6763,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>546840</xdr:colOff>
+      <xdr:colOff>573840</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>145080</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>615240</xdr:colOff>
+      <xdr:colOff>641880</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6781,8 +6779,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16697160" y="9410760"/>
-        <a:ext cx="2507040" cy="1403280"/>
+        <a:off x="16724160" y="9401760"/>
+        <a:ext cx="2506680" cy="1402920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6795,15 +6793,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>703440</xdr:colOff>
+      <xdr:colOff>730440</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>67320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6811,8 +6809,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16853760" y="13394880"/>
-        <a:ext cx="2615040" cy="1411560"/>
+        <a:off x="16880760" y="13385880"/>
+        <a:ext cx="2614680" cy="1411200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6825,15 +6823,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>112680</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>652680</xdr:colOff>
+      <xdr:colOff>679320</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6841,8 +6839,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11359440" y="9424440"/>
-        <a:ext cx="2192400" cy="1462320"/>
+        <a:off x="11386440" y="9415440"/>
+        <a:ext cx="2192040" cy="1461960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6855,15 +6853,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>101520</xdr:colOff>
+      <xdr:colOff>128520</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>734400</xdr:colOff>
+      <xdr:colOff>761040</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6871,8 +6869,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11375280" y="13309200"/>
-        <a:ext cx="2258280" cy="1475640"/>
+        <a:off x="11402280" y="13300200"/>
+        <a:ext cx="2257920" cy="1475280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6885,15 +6883,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>579960</xdr:colOff>
+      <xdr:colOff>606960</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>477720</xdr:colOff>
+      <xdr:colOff>504360</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6901,8 +6899,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8602200" y="9451080"/>
-        <a:ext cx="2336400" cy="1340640"/>
+        <a:off x="8629200" y="9442080"/>
+        <a:ext cx="2336040" cy="1340280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6915,15 +6913,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>753840</xdr:colOff>
+      <xdr:colOff>780840</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>556200</xdr:colOff>
+      <xdr:colOff>582840</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6931,8 +6929,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8776080" y="13417200"/>
-        <a:ext cx="2241000" cy="1371960"/>
+        <a:off x="8803080" y="13408200"/>
+        <a:ext cx="2240640" cy="1371600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6945,15 +6943,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>233640</xdr:colOff>
+      <xdr:colOff>260640</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>343080</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:colOff>369720</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6961,8 +6959,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5817600" y="9559800"/>
-        <a:ext cx="2547720" cy="1500120"/>
+        <a:off x="5844600" y="9550800"/>
+        <a:ext cx="2547360" cy="1499760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6975,15 +6973,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>364680</xdr:colOff>
+      <xdr:colOff>391680</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>250920</xdr:colOff>
+      <xdr:colOff>277560</xdr:colOff>
       <xdr:row>91</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6991,8 +6989,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5948640" y="13512240"/>
-        <a:ext cx="2324520" cy="1304280"/>
+        <a:off x="5975640" y="13503240"/>
+        <a:ext cx="2324160" cy="1303920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7005,15 +7003,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>111960</xdr:colOff>
+      <xdr:colOff>138960</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7021,8 +7019,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11385720" y="11308320"/>
-        <a:ext cx="2431800" cy="1458360"/>
+        <a:off x="11412720" y="11299320"/>
+        <a:ext cx="2431440" cy="1458000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7035,15 +7033,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>684720</xdr:colOff>
+      <xdr:colOff>711720</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>618480</xdr:colOff>
+      <xdr:colOff>645120</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7051,8 +7049,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8706960" y="11304000"/>
-        <a:ext cx="2372400" cy="1447920"/>
+        <a:off x="8733960" y="11295000"/>
+        <a:ext cx="2372040" cy="1447560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7065,15 +7063,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>373680</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:colOff>400680</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>415080</xdr:colOff>
+      <xdr:colOff>441720</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7081,8 +7079,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5957640" y="11385720"/>
-        <a:ext cx="2479680" cy="1285560"/>
+        <a:off x="5984640" y="11376720"/>
+        <a:ext cx="2479320" cy="1285200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7095,15 +7093,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>102960</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>339120</xdr:colOff>
+      <xdr:colOff>365760</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7111,8 +7109,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17039160" y="11466720"/>
-        <a:ext cx="2701440" cy="1531800"/>
+        <a:off x="17066160" y="11457720"/>
+        <a:ext cx="2701080" cy="1531440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7125,15 +7123,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>140400</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>167400</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>457920</xdr:colOff>
+      <xdr:colOff>484560</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7141,8 +7139,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13852440" y="11385360"/>
-        <a:ext cx="2755800" cy="1454400"/>
+        <a:off x="13879440" y="11376360"/>
+        <a:ext cx="2755440" cy="1454040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7155,15 +7153,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>742320</xdr:colOff>
+      <xdr:colOff>769320</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>776160</xdr:colOff>
+      <xdr:colOff>802800</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7171,8 +7169,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6326280" y="7764480"/>
-        <a:ext cx="2472120" cy="1412640"/>
+        <a:off x="6353280" y="7755480"/>
+        <a:ext cx="2471760" cy="1412280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7185,15 +7183,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>295560</xdr:colOff>
+      <xdr:colOff>322200</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7201,8 +7199,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9047160" y="7778880"/>
-        <a:ext cx="2522160" cy="1344600"/>
+        <a:off x="9074160" y="7769880"/>
+        <a:ext cx="2521800" cy="1344240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7215,15 +7213,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>142560</xdr:colOff>
+      <xdr:colOff>169560</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>306720</xdr:colOff>
+      <xdr:colOff>333360</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7231,8 +7229,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11416320" y="7761600"/>
-        <a:ext cx="2602440" cy="1413000"/>
+        <a:off x="11443320" y="7752600"/>
+        <a:ext cx="2602080" cy="1412640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7245,15 +7243,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>271800</xdr:colOff>
+      <xdr:colOff>298800</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>577800</xdr:colOff>
+      <xdr:colOff>604440</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7261,8 +7259,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13983840" y="7823160"/>
-        <a:ext cx="2744280" cy="1398240"/>
+        <a:off x="14010840" y="7814160"/>
+        <a:ext cx="2743920" cy="1397880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7275,15 +7273,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>442800</xdr:colOff>
+      <xdr:colOff>469800</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>573480</xdr:colOff>
+      <xdr:colOff>600120</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7291,8 +7289,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16593120" y="7734600"/>
-        <a:ext cx="2569320" cy="1506960"/>
+        <a:off x="16620120" y="7725600"/>
+        <a:ext cx="2568960" cy="1506600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7310,10 +7308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:V88"/>
+  <dimension ref="A2:V103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H80" activeCellId="0" sqref="H80"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H99" activeCellId="0" sqref="H99:H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8775,6 +8773,141 @@
       <c r="H88" s="1" t="n">
         <f aca="false">SUM(H83:H87)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="22" t="n">
+        <f aca="false">(D62-D72)/D$62</f>
+        <v>0.00515463917525774</v>
+      </c>
+      <c r="E92" s="22" t="n">
+        <f aca="false">(E62-E72)/E$62</f>
+        <v>0.00793650793650794</v>
+      </c>
+      <c r="F92" s="22" t="n">
+        <f aca="false">(F62-F72)/F$62</f>
+        <v>0.60625</v>
+      </c>
+      <c r="G92" s="22" t="n">
+        <f aca="false">(G62-G72)/G$62</f>
+        <v>-0.0436300174520068</v>
+      </c>
+      <c r="H92" s="22" t="n">
+        <f aca="false">(H62-H72)/H$62</f>
+        <v>-0.0368098159509203</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="22" t="n">
+        <f aca="false">(D63-D73)/D$63</f>
+        <v>0.0635593220338984</v>
+      </c>
+      <c r="E93" s="22" t="n">
+        <f aca="false">(E63-E73)/E$63</f>
+        <v>0.611940298507463</v>
+      </c>
+      <c r="F93" s="22" t="n">
+        <f aca="false">(F63-F73)/F$63</f>
+        <v>0.602209944751381</v>
+      </c>
+      <c r="G93" s="22" t="n">
+        <f aca="false">(G63-G73)/G$63</f>
+        <v>-0.0185185185185185</v>
+      </c>
+      <c r="H93" s="22" t="n">
+        <f aca="false">(H63-H73)/H$63</f>
+        <v>0.0149892933618844</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="22" t="n">
+        <f aca="false">(D64-D74)/D$64</f>
+        <v>0.597457627118644</v>
+      </c>
+      <c r="E94" s="22" t="n">
+        <f aca="false">(E64-E74)/E$64</f>
+        <v>0.592307692307692</v>
+      </c>
+      <c r="F94" s="22" t="n">
+        <f aca="false">(F64-F74)/F$64</f>
+        <v>0.586206896551724</v>
+      </c>
+      <c r="G94" s="22" t="n">
+        <f aca="false">(G64-G74)/G$64</f>
+        <v>0.525</v>
+      </c>
+      <c r="H94" s="22" t="n">
+        <f aca="false">(H64-H74)/H$64</f>
+        <v>0.533333333333333</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="22" t="n">
+        <f aca="false">(D65-D75)/D$65</f>
+        <v>0.011764705882353</v>
+      </c>
+      <c r="E95" s="22" t="n">
+        <f aca="false">(E65-E75)/E$65</f>
+        <v>-0.00813008130081302</v>
+      </c>
+      <c r="F95" s="22" t="n">
+        <f aca="false">(F65-F75)/F$65</f>
+        <v>0.0144927536231884</v>
+      </c>
+      <c r="G95" s="22" t="n">
+        <f aca="false">(G65-G75)/G$65</f>
+        <v>0.397590361445783</v>
+      </c>
+      <c r="H95" s="22" t="n">
+        <f aca="false">(H65-H75)/H$65</f>
+        <v>0.113207547169811</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H99" s="0" t="n">
+        <f aca="false">(H62-H72)/H62</f>
+        <v>-0.0368098159509203</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H100" s="0" t="n">
+        <f aca="false">(H63-H73)/H63</f>
+        <v>0.0149892933618844</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H101" s="0" t="n">
+        <f aca="false">(H64-H74)/H64</f>
+        <v>0.533333333333333</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H102" s="0" t="n">
+        <f aca="false">(H65-H75)/H65</f>
+        <v>0.113207547169811</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H103" s="0" t="n">
+        <f aca="false">(H66-H76)/H66</f>
+        <v>0.55</v>
       </c>
     </row>
   </sheetData>
@@ -8801,7 +8934,7 @@
   <dimension ref="A1:AP98"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="1" sqref="H99:H103 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8812,42 +8945,42 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="n">
+      <c r="B3" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C3" s="7" t="n">
@@ -8865,12 +8998,12 @@
       <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -8890,12 +9023,12 @@
         <v>0.55</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -8915,12 +9048,12 @@
       <c r="G5" s="2" t="n">
         <v>0.59</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -8934,12 +9067,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -8955,12 +9088,12 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -8976,12 +9109,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -8995,12 +9128,12 @@
       <c r="G9" s="2" t="n">
         <v>1.02</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -9014,12 +9147,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -9031,118 +9164,118 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="I16" s="22" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="I16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="P16" s="22" t="s">
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="P16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="W16" s="22" t="s">
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="W16" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-      <c r="AD16" s="22" t="s">
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AD16" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AI16" s="22"/>
-      <c r="AK16" s="22" t="s">
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="23"/>
+      <c r="AG16" s="23"/>
+      <c r="AH16" s="23"/>
+      <c r="AI16" s="23"/>
+      <c r="AK16" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AL16" s="22"/>
-      <c r="AM16" s="22"/>
-      <c r="AN16" s="22"/>
-      <c r="AO16" s="22"/>
-      <c r="AP16" s="22"/>
+      <c r="AL16" s="23"/>
+      <c r="AM16" s="23"/>
+      <c r="AN16" s="23"/>
+      <c r="AO16" s="23"/>
+      <c r="AP16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="I17" s="24" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="I17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="P17" s="24" t="s">
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="P17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="W17" s="24" t="s">
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="W17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AD17" s="24" t="s">
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AD17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-      <c r="AG17" s="24"/>
-      <c r="AH17" s="24"/>
-      <c r="AI17" s="24"/>
-      <c r="AK17" s="24" t="s">
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AK17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AL17" s="24"/>
-      <c r="AM17" s="24"/>
-      <c r="AN17" s="24"/>
-      <c r="AO17" s="24"/>
-      <c r="AP17" s="24"/>
+      <c r="AL17" s="25"/>
+      <c r="AM17" s="25"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="n">
+      <c r="B18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C18" s="7" t="n">
@@ -9160,7 +9293,7 @@
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="25" t="n">
+      <c r="I18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="J18" s="7" t="n">
@@ -9178,7 +9311,7 @@
       <c r="N18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P18" s="25" t="n">
+      <c r="P18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="Q18" s="7" t="n">
@@ -9196,7 +9329,7 @@
       <c r="U18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="W18" s="25" t="n">
+      <c r="W18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="X18" s="7" t="n">
@@ -9214,7 +9347,7 @@
       <c r="AB18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AD18" s="25" t="n">
+      <c r="AD18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="AE18" s="7" t="n">
@@ -9232,7 +9365,7 @@
       <c r="AI18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AK18" s="25" t="n">
+      <c r="AK18" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="AL18" s="7" t="n">
@@ -9675,30 +9808,30 @@
       <c r="AP27" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="25" t="n">
+      <c r="B32" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C32" s="7" t="n">
@@ -9722,12 +9855,12 @@
         <v>3</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9735,10 +9868,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9746,10 +9879,10 @@
         <v>5</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9757,10 +9890,10 @@
         <v>6</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9768,10 +9901,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9779,10 +9912,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9790,10 +9923,10 @@
         <v>9</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9801,10 +9934,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9812,53 +9945,53 @@
         <v>37</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
       <c r="G41" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="I44" s="22" t="s">
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="I44" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="I45" s="30" t="s">
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="I45" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="25" t="n">
+      <c r="B46" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C46" s="7" t="n">
@@ -9876,12 +10009,12 @@
       <c r="G46" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -9902,11 +10035,11 @@
       </c>
       <c r="G47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
-      <c r="N47" s="28"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -9927,11 +10060,11 @@
         <v>405</v>
       </c>
       <c r="I48" s="2"/>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="28"/>
-      <c r="N48" s="28"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -9946,11 +10079,11 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -9967,11 +10100,11 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="I50" s="2"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -9988,11 +10121,11 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="28"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -10007,11 +10140,11 @@
         <v>560</v>
       </c>
       <c r="I52" s="2"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="28"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -10026,11 +10159,11 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="28"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -10043,11 +10176,11 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
@@ -10067,110 +10200,110 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="I59" s="22" t="s">
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="I59" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="P59" s="22" t="s">
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
+      <c r="P59" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
-      <c r="S59" s="22"/>
-      <c r="T59" s="22"/>
-      <c r="U59" s="22"/>
-      <c r="W59" s="22" t="s">
+      <c r="Q59" s="23"/>
+      <c r="R59" s="23"/>
+      <c r="S59" s="23"/>
+      <c r="T59" s="23"/>
+      <c r="U59" s="23"/>
+      <c r="W59" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="X59" s="22"/>
-      <c r="Y59" s="22"/>
-      <c r="Z59" s="22"/>
-      <c r="AA59" s="22"/>
-      <c r="AB59" s="22"/>
-      <c r="AD59" s="22" t="s">
+      <c r="X59" s="23"/>
+      <c r="Y59" s="23"/>
+      <c r="Z59" s="23"/>
+      <c r="AA59" s="23"/>
+      <c r="AB59" s="23"/>
+      <c r="AD59" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AE59" s="22"/>
-      <c r="AF59" s="22"/>
-      <c r="AG59" s="22"/>
-      <c r="AH59" s="22"/>
-      <c r="AI59" s="22"/>
-      <c r="AK59" s="22" t="s">
+      <c r="AE59" s="23"/>
+      <c r="AF59" s="23"/>
+      <c r="AG59" s="23"/>
+      <c r="AH59" s="23"/>
+      <c r="AI59" s="23"/>
+      <c r="AK59" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AL59" s="22"/>
-      <c r="AM59" s="22"/>
-      <c r="AN59" s="22"/>
-      <c r="AO59" s="22"/>
-      <c r="AP59" s="22"/>
+      <c r="AL59" s="23"/>
+      <c r="AM59" s="23"/>
+      <c r="AN59" s="23"/>
+      <c r="AO59" s="23"/>
+      <c r="AP59" s="23"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="I60" s="24" t="s">
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="I60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="24"/>
-      <c r="P60" s="24" t="s">
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="25"/>
+      <c r="P60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q60" s="24"/>
-      <c r="R60" s="24"/>
-      <c r="S60" s="24"/>
-      <c r="T60" s="24"/>
-      <c r="U60" s="24"/>
-      <c r="W60" s="24" t="s">
+      <c r="Q60" s="25"/>
+      <c r="R60" s="25"/>
+      <c r="S60" s="25"/>
+      <c r="T60" s="25"/>
+      <c r="U60" s="25"/>
+      <c r="W60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="X60" s="24"/>
-      <c r="Y60" s="24"/>
-      <c r="Z60" s="24"/>
-      <c r="AA60" s="24"/>
-      <c r="AB60" s="24"/>
-      <c r="AD60" s="24" t="s">
+      <c r="X60" s="25"/>
+      <c r="Y60" s="25"/>
+      <c r="Z60" s="25"/>
+      <c r="AA60" s="25"/>
+      <c r="AB60" s="25"/>
+      <c r="AD60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AE60" s="24"/>
-      <c r="AF60" s="24"/>
-      <c r="AG60" s="24"/>
-      <c r="AH60" s="24"/>
-      <c r="AI60" s="24"/>
-      <c r="AK60" s="24" t="s">
+      <c r="AE60" s="25"/>
+      <c r="AF60" s="25"/>
+      <c r="AG60" s="25"/>
+      <c r="AH60" s="25"/>
+      <c r="AI60" s="25"/>
+      <c r="AK60" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="AL60" s="24"/>
-      <c r="AM60" s="24"/>
-      <c r="AN60" s="24"/>
-      <c r="AO60" s="24"/>
-      <c r="AP60" s="24"/>
+      <c r="AL60" s="25"/>
+      <c r="AM60" s="25"/>
+      <c r="AN60" s="25"/>
+      <c r="AO60" s="25"/>
+      <c r="AP60" s="25"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="25" t="n">
+      <c r="B61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C61" s="7" t="n">
@@ -10188,7 +10321,7 @@
       <c r="G61" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I61" s="25" t="n">
+      <c r="I61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="J61" s="7" t="n">
@@ -10206,7 +10339,7 @@
       <c r="N61" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P61" s="25" t="n">
+      <c r="P61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="Q61" s="7" t="n">
@@ -10224,7 +10357,7 @@
       <c r="U61" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="W61" s="25" t="n">
+      <c r="W61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="X61" s="7" t="n">
@@ -10242,7 +10375,7 @@
       <c r="AB61" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AD61" s="25" t="n">
+      <c r="AD61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="AE61" s="7" t="n">
@@ -10260,7 +10393,7 @@
       <c r="AI61" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AK61" s="25" t="n">
+      <c r="AK61" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="AL61" s="7" t="n">
@@ -10295,11 +10428,11 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="I62" s="25" t="s">
+      <c r="I62" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J62" s="2"/>
-      <c r="K62" s="25" t="s">
+      <c r="K62" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L62" s="2"/>
@@ -10346,11 +10479,11 @@
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="I63" s="25" t="s">
+      <c r="I63" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J63" s="2"/>
-      <c r="K63" s="25" t="s">
+      <c r="K63" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L63" s="2"/>
@@ -10397,11 +10530,11 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="I64" s="25" t="s">
+      <c r="I64" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J64" s="2"/>
-      <c r="K64" s="25" t="s">
+      <c r="K64" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L64" s="2"/>
@@ -10448,11 +10581,11 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="I65" s="25" t="s">
+      <c r="I65" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J65" s="2"/>
-      <c r="K65" s="25" t="s">
+      <c r="K65" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L65" s="2"/>
@@ -10499,11 +10632,11 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="I66" s="25" t="s">
+      <c r="I66" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J66" s="2"/>
-      <c r="K66" s="25" t="s">
+      <c r="K66" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L66" s="2"/>
@@ -10550,11 +10683,11 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="I67" s="25" t="s">
+      <c r="I67" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J67" s="2"/>
-      <c r="K67" s="25" t="s">
+      <c r="K67" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L67" s="2"/>
@@ -10601,11 +10734,11 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="I68" s="25" t="s">
+      <c r="I68" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J68" s="2"/>
-      <c r="K68" s="25" t="s">
+      <c r="K68" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L68" s="2"/>
@@ -10652,11 +10785,11 @@
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="I69" s="25" t="s">
+      <c r="I69" s="26" t="s">
         <v>42</v>
       </c>
       <c r="J69" s="2"/>
-      <c r="K69" s="25" t="s">
+      <c r="K69" s="26" t="s">
         <v>42</v>
       </c>
       <c r="L69" s="2"/>
@@ -10753,34 +10886,34 @@
       <c r="AP70" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-      <c r="G73" s="22"/>
-      <c r="I73" s="22" t="s">
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="I73" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="K73" s="31" t="s">
+      <c r="K73" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="24" t="s">
+      <c r="B74" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
-      <c r="I74" s="30" t="s">
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="I74" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="K74" s="32" t="s">
+      <c r="K74" s="33" t="s">
         <v>46</v>
       </c>
     </row>
@@ -10788,7 +10921,7 @@
       <c r="A75" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="25" t="n">
+      <c r="B75" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C75" s="7" t="n">
@@ -10815,14 +10948,14 @@
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="33" t="s">
+      <c r="B76" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
       <c r="I76" s="2" t="n">
         <v>29.69</v>
       </c>
@@ -10834,12 +10967,12 @@
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="34"/>
+      <c r="G77" s="34"/>
       <c r="I77" s="2" t="n">
         <v>41.38</v>
       </c>
@@ -10851,12 +10984,12 @@
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="34"/>
+      <c r="G78" s="34"/>
       <c r="I78" s="2" t="n">
         <v>11.54</v>
       </c>
@@ -10868,12 +11001,12 @@
       <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="33"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
       <c r="I79" s="2" t="n">
         <v>3.84</v>
       </c>
@@ -10885,16 +11018,16 @@
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
-      <c r="I80" s="34" t="n">
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="I80" s="35" t="n">
         <v>13.54</v>
       </c>
-      <c r="K80" s="34" t="n">
+      <c r="K80" s="35" t="n">
         <v>2.19</v>
       </c>
     </row>
@@ -10902,79 +11035,79 @@
       <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="33"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
-      <c r="I81" s="34"/>
-      <c r="K81" s="34"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="34"/>
+      <c r="G81" s="34"/>
+      <c r="I81" s="35"/>
+      <c r="K81" s="35"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="33"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
-      <c r="I82" s="34"/>
-      <c r="K82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="34"/>
+      <c r="I82" s="35"/>
+      <c r="K82" s="35"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B83" s="33"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="33"/>
-      <c r="I83" s="34"/>
-      <c r="K83" s="34"/>
+      <c r="B83" s="34"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="34"/>
+      <c r="G83" s="34"/>
+      <c r="I83" s="35"/>
+      <c r="K83" s="35"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B84" s="33"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="33"/>
-      <c r="F84" s="33"/>
-      <c r="G84" s="33"/>
+      <c r="B84" s="34"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="34"/>
       <c r="I84" s="7"/>
       <c r="K84" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="24" t="s">
+      <c r="B88" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="25"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B89" s="25" t="n">
+      <c r="B89" s="26" t="n">
         <v>2859</v>
       </c>
       <c r="C89" s="7" t="n">
@@ -10997,102 +11130,102 @@
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B90" s="33" t="s">
+      <c r="B90" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B91" s="33"/>
-      <c r="C91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="33"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="33"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="34"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="34"/>
+      <c r="G91" s="34"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B92" s="33"/>
-      <c r="C92" s="33"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="34"/>
+      <c r="G92" s="34"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="33"/>
-      <c r="C93" s="33"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="33"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="34"/>
+      <c r="G93" s="34"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="33"/>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="33"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="34"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="34"/>
+      <c r="G94" s="34"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="33"/>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
-      <c r="F95" s="33"/>
-      <c r="G95" s="33"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="34"/>
+      <c r="G95" s="34"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B96" s="33"/>
-      <c r="C96" s="33"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="33"/>
-      <c r="F96" s="33"/>
-      <c r="G96" s="33"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="34"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="34"/>
+      <c r="F96" s="34"/>
+      <c r="G96" s="34"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="33"/>
-      <c r="C97" s="33"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="33"/>
-      <c r="F97" s="33"/>
-      <c r="G97" s="33"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="34"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="34"/>
+      <c r="G97" s="34"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B98" s="33"/>
-      <c r="C98" s="33"/>
-      <c r="D98" s="33"/>
-      <c r="E98" s="33"/>
-      <c r="F98" s="33"/>
-      <c r="G98" s="33"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>